<commit_message>
arrumando sql injection da agenda 3.0
</commit_message>
<xml_diff>
--- a/UC_6/planilha/testes-agendavinitopgod.xlsx
+++ b/UC_6/planilha/testes-agendavinitopgod.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinicius.svsantos\Documents\tecnicoInformaticaSenac\UC_6\planilha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinicius.svsantos\Documents\GITHUB\tecnicoInformaticaSenac\UC_6\planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="2"/>
+    <workbookView minimized="1" xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Banco dados" sheetId="1" r:id="rId1"/>
@@ -407,6 +407,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -427,13 +434,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,7 +737,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -745,28 +745,28 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="9"/>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="9"/>
       <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="9"/>
       <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="9"/>
       <c r="B6" t="s">
         <v>23</v>
       </c>
@@ -775,7 +775,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="9"/>
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -784,7 +784,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="9"/>
       <c r="B8" t="s">
         <v>27</v>
       </c>
@@ -817,19 +817,19 @@
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>22</v>
       </c>
@@ -838,7 +838,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>23</v>
       </c>
@@ -847,17 +847,17 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -874,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
@@ -909,42 +909,42 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8" t="s">
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8" t="s">
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -1007,7 +1007,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -1070,19 +1070,19 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="10"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="10"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="10"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="10"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1127,7 +1127,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
@@ -1159,7 +1159,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="12"/>
       <c r="B3" t="s">
         <v>48</v>
       </c>
@@ -1189,7 +1189,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="12"/>
       <c r="B4" t="s">
         <v>56</v>
       </c>
@@ -1219,7 +1219,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="12"/>
       <c r="B5" t="s">
         <v>62</v>
       </c>
@@ -1249,7 +1249,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="12"/>
       <c r="B6" t="s">
         <v>71</v>
       </c>
@@ -1385,7 +1385,7 @@
       <c r="F10" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="6" t="s">
         <v>91</v>
       </c>
       <c r="H10" t="s">
@@ -1428,7 +1428,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H12" s="15"/>
+      <c r="H12" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1453,31 +1453,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="8" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="9"/>
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -1487,17 +1487,17 @@
       <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="12"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="9"/>
       <c r="B4" t="s">
         <v>31</v>
       </c>
@@ -1515,10 +1515,10 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="9"/>
       <c r="L6" s="5"/>
     </row>
   </sheetData>

</xml_diff>